<commit_message>
submit result for lesson 20
</commit_message>
<xml_diff>
--- a/19-Discrete Choice/LogitModelApplication.xlsx
+++ b/19-Discrete Choice/LogitModelApplication.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdulaziz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdulaziz/Desktop/UK_courses/CE599/ce599/19-Discrete Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="28940" yWindow="460" windowWidth="25600" windowHeight="20860"/>
   </bookViews>
   <sheets>
     <sheet name="model 1" sheetId="1" r:id="rId1"/>
@@ -63,10 +63,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,8 +126,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -120,7 +144,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -765,5 +797,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>